<commit_message>
method uniqueAbilityReturnDamage() in class BattleTech() returns tuple (damageType = '', damageVolume = 0). For classes Gladiator & Inferno this method is overriden according to the doc-string info in class BattleTech. Now attribute TechType in class BattleTech() and its instances cannot be reset by its named 'Setter' cause it has been commented (disabled).
</commit_message>
<xml_diff>
--- a/TestBattleResults/1_BattlesResults.xlsx
+++ b/TestBattleResults/1_BattlesResults.xlsx
@@ -70,10 +70,10 @@
     <t>Sparky</t>
   </si>
   <si>
+    <t>Zeus</t>
+  </si>
+  <si>
     <t>Hornet</t>
-  </si>
-  <si>
-    <t>Zeus</t>
   </si>
   <si>
     <t>Scout</t>
@@ -528,7 +528,7 @@
         <v>999</v>
       </c>
       <c r="J2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -537,13 +537,13 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>401.48</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>681.8</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -575,7 +575,7 @@
         <v>666</v>
       </c>
       <c r="J3">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -584,13 +584,13 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>21.49</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>64.34999999999999</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -622,16 +622,16 @@
         <v>499</v>
       </c>
       <c r="J4">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="K4">
-        <v>104.09</v>
+        <v>349.83</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>227.15</v>
+        <v>329.3</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -654,22 +654,22 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5">
         <v>700</v>
       </c>
       <c r="G5">
-        <v>355</v>
+        <v>900</v>
       </c>
       <c r="H5">
         <v>599</v>
       </c>
       <c r="I5">
-        <v>599</v>
+        <v>499</v>
       </c>
       <c r="J5">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>418.6</v>
+        <v>297.63</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -701,22 +701,22 @@
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>700</v>
       </c>
       <c r="G6">
-        <v>900</v>
+        <v>355</v>
       </c>
       <c r="H6">
         <v>599</v>
       </c>
       <c r="I6">
-        <v>499</v>
+        <v>599</v>
       </c>
       <c r="J6">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -725,13 +725,13 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>194.61</v>
       </c>
       <c r="N6">
-        <v>427.31</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -763,7 +763,7 @@
         <v>499</v>
       </c>
       <c r="J7">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -810,7 +810,7 @@
         <v>666</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>176.83</v>
+        <v>214.4</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -857,7 +857,7 @@
         <v>499</v>
       </c>
       <c r="J9">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>530</v>
+        <v>544.73</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -889,37 +889,37 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F10">
         <v>299</v>
       </c>
       <c r="G10">
-        <v>355</v>
+        <v>900</v>
       </c>
       <c r="H10">
         <v>999</v>
       </c>
       <c r="I10">
-        <v>599</v>
+        <v>499</v>
       </c>
       <c r="J10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>877.71</v>
       </c>
       <c r="N10">
-        <v>514.0599999999999</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -936,22 +936,22 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>299</v>
       </c>
       <c r="G11">
-        <v>900</v>
+        <v>355</v>
       </c>
       <c r="H11">
         <v>999</v>
       </c>
       <c r="I11">
-        <v>499</v>
+        <v>599</v>
       </c>
       <c r="J11">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>18.94</v>
+        <v>234.67</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -998,7 +998,7 @@
         <v>499</v>
       </c>
       <c r="J12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>463.26</v>
+        <v>398.66</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1045,16 +1045,16 @@
         <v>499</v>
       </c>
       <c r="J13">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K13">
-        <v>256.57</v>
+        <v>48.9</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>666</v>
+        <v>317.1</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -1077,31 +1077,31 @@
         <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F14">
         <v>666</v>
       </c>
       <c r="G14">
-        <v>355</v>
+        <v>900</v>
       </c>
       <c r="H14">
         <v>666</v>
       </c>
       <c r="I14">
-        <v>599</v>
+        <v>499</v>
       </c>
       <c r="J14">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K14">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>401.62</v>
+        <v>404.49</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1124,22 +1124,22 @@
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F15">
         <v>666</v>
       </c>
       <c r="G15">
-        <v>900</v>
+        <v>355</v>
       </c>
       <c r="H15">
         <v>666</v>
       </c>
       <c r="I15">
-        <v>499</v>
+        <v>599</v>
       </c>
       <c r="J15">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>500.36</v>
+        <v>530.46</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -1186,16 +1186,16 @@
         <v>499</v>
       </c>
       <c r="J16">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>481.59</v>
+        <v>172.67</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -1218,22 +1218,22 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F17">
         <v>500</v>
       </c>
       <c r="G17">
-        <v>355</v>
+        <v>900</v>
       </c>
       <c r="H17">
         <v>499</v>
       </c>
       <c r="I17">
-        <v>599</v>
+        <v>499</v>
       </c>
       <c r="J17">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1245,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>232.15</v>
+        <v>216.92</v>
       </c>
       <c r="O17">
         <v>2</v>
@@ -1265,37 +1265,37 @@
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>500</v>
       </c>
       <c r="G18">
-        <v>900</v>
+        <v>355</v>
       </c>
       <c r="H18">
         <v>499</v>
       </c>
       <c r="I18">
-        <v>499</v>
+        <v>599</v>
       </c>
       <c r="J18">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="K18">
-        <v>35.63</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>688.08</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>499</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>147.43</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1327,22 +1327,22 @@
         <v>499</v>
       </c>
       <c r="J19">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="K19">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>64.26000000000001</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>173.43</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>214.15</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1356,40 +1356,40 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
         <v>24</v>
       </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
       <c r="F20">
+        <v>900</v>
+      </c>
+      <c r="G20">
         <v>355</v>
       </c>
-      <c r="G20">
-        <v>900</v>
-      </c>
       <c r="H20">
+        <v>499</v>
+      </c>
+      <c r="I20">
         <v>599</v>
       </c>
-      <c r="I20">
-        <v>499</v>
-      </c>
       <c r="J20">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K20">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>24.63</v>
       </c>
       <c r="M20">
-        <v>168.12</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>47.53</v>
       </c>
       <c r="O20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1403,40 +1403,40 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21">
-        <v>355</v>
+        <v>900</v>
       </c>
       <c r="G21">
         <v>300</v>
       </c>
       <c r="H21">
-        <v>599</v>
+        <v>499</v>
       </c>
       <c r="I21">
         <v>499</v>
       </c>
       <c r="J21">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>138.36</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>499</v>
       </c>
       <c r="N21">
-        <v>207.67</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1450,25 +1450,25 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22">
-        <v>900</v>
+        <v>355</v>
       </c>
       <c r="G22">
         <v>300</v>
       </c>
       <c r="H22">
-        <v>499</v>
+        <v>599</v>
       </c>
       <c r="I22">
         <v>499</v>
       </c>
       <c r="J22">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1477,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <v>270.03</v>
+        <v>308.01</v>
       </c>
       <c r="N22">
         <v>0</v>

</xml_diff>